<commit_message>
Bug fixes, upgrade openpyxl
</commit_message>
<xml_diff>
--- a/cmbautomiser/ods_templates/dev.xlsx
+++ b/cmbautomiser/ods_templates/dev.xlsx
@@ -1,16 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\HP\cmbautomiser\cmbautomiser\ods_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123E660D-7D8C-4055-A96A-69C1CA6899F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="start" sheetId="1" r:id="rId1"/>
     <sheet name="end" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -147,12 +162,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$₹-4009]#,##0;\-[$₹-4009]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +544,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -575,7 +598,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,9 +630,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,6 +682,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -816,33 +875,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="10" width="10.140625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
-    <col min="19" max="1025" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="9" max="10" width="10.109375" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="1" customWidth="1"/>
+    <col min="19" max="1025" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -863,7 +922,7 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -883,7 +942,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -914,7 +973,7 @@
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -937,7 +996,7 @@
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -960,7 +1019,7 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
@@ -983,7 +1042,7 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1068,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="5"/>
@@ -1029,7 +1088,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="35"/>
@@ -1055,7 +1114,7 @@
       <c r="Q9" s="35"/>
       <c r="R9" s="35"/>
     </row>
-    <row r="10" spans="1:18" ht="60">
+    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="43">
         <v>1</v>
       </c>
@@ -1174,23 +1233,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="1" customWidth="1"/>
-    <col min="18" max="1025" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="1" customWidth="1"/>
+    <col min="4" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" style="1" customWidth="1"/>
+    <col min="18" max="1025" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45"/>
       <c r="B1" s="45"/>
       <c r="C1" s="46" t="s">
@@ -1214,7 +1273,7 @@
       <c r="Q1" s="52"/>
       <c r="R1" s="53"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickTop="1">
+    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="54" t="s">
@@ -1241,7 +1300,7 @@
       </c>
       <c r="R2" s="61"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="62"/>
       <c r="B3" s="62"/>
       <c r="C3" s="54" t="s">

</xml_diff>